<commit_message>
Added log log plots
</commit_message>
<xml_diff>
--- a/covid_19_data_switzerland.xlsx
+++ b/covid_19_data_switzerland.xlsx
@@ -987,7 +987,9 @@
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
       <c r="U11" t="inlineStr"/>
-      <c r="V11" t="inlineStr"/>
+      <c r="V11" t="n">
+        <v>18</v>
+      </c>
       <c r="W11" t="inlineStr"/>
       <c r="X11" t="inlineStr"/>
       <c r="Y11" t="n">
@@ -1000,7 +1002,7 @@
         <v>19</v>
       </c>
       <c r="AB11" t="n">
-        <v>87</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12">
@@ -1060,7 +1062,7 @@
         <v>26</v>
       </c>
       <c r="AB12" t="n">
-        <v>149</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13">
@@ -1097,7 +1099,9 @@
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
       <c r="U13" t="inlineStr"/>
-      <c r="V13" t="inlineStr"/>
+      <c r="V13" t="n">
+        <v>45</v>
+      </c>
       <c r="W13" t="inlineStr"/>
       <c r="X13" t="n">
         <v>30</v>
@@ -1108,7 +1112,7 @@
         <v>30</v>
       </c>
       <c r="AB13" t="n">
-        <v>185</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14">
@@ -1147,7 +1151,9 @@
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
-      <c r="V14" t="inlineStr"/>
+      <c r="V14" t="n">
+        <v>58</v>
+      </c>
       <c r="W14" t="inlineStr"/>
       <c r="X14" t="n">
         <v>40</v>
@@ -1160,7 +1166,7 @@
         <v>37</v>
       </c>
       <c r="AB14" t="n">
-        <v>221</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15">
@@ -1205,7 +1211,9 @@
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr"/>
       <c r="U15" t="inlineStr"/>
-      <c r="V15" t="inlineStr"/>
+      <c r="V15" t="n">
+        <v>68</v>
+      </c>
       <c r="W15" t="inlineStr"/>
       <c r="X15" t="n">
         <v>51</v>
@@ -1218,7 +1226,7 @@
         <v>40</v>
       </c>
       <c r="AB15" t="n">
-        <v>278</v>
+        <v>341</v>
       </c>
     </row>
     <row r="16">
@@ -1270,7 +1278,7 @@
         <v>49</v>
       </c>
       <c r="AB16" t="n">
-        <v>353</v>
+        <v>416</v>
       </c>
     </row>
     <row r="17">
@@ -1326,7 +1334,7 @@
         <v>59</v>
       </c>
       <c r="AB17" t="n">
-        <v>440</v>
+        <v>503</v>
       </c>
     </row>
     <row r="18">
@@ -2888,8 +2896,12 @@
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
-      <c r="C39" t="inlineStr"/>
-      <c r="D39" t="inlineStr"/>
+      <c r="C39" t="n">
+        <v>19</v>
+      </c>
+      <c r="D39" t="n">
+        <v>63</v>
+      </c>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr"/>
@@ -2903,7 +2915,9 @@
       <c r="O39" t="inlineStr"/>
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr"/>
-      <c r="R39" t="inlineStr"/>
+      <c r="R39" t="n">
+        <v>44</v>
+      </c>
       <c r="S39" t="inlineStr"/>
       <c r="T39" t="inlineStr"/>
       <c r="U39" t="inlineStr"/>
@@ -2911,10 +2925,12 @@
       <c r="W39" t="inlineStr"/>
       <c r="X39" t="inlineStr"/>
       <c r="Y39" t="inlineStr"/>
-      <c r="Z39" t="inlineStr"/>
+      <c r="Z39" t="n">
+        <v>131</v>
+      </c>
       <c r="AA39" t="inlineStr"/>
       <c r="AB39" t="n">
-        <v>17768</v>
+        <v>17781</v>
       </c>
     </row>
   </sheetData>
@@ -4972,7 +4988,9 @@
       </c>
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr"/>
-      <c r="D39" t="inlineStr"/>
+      <c r="D39" t="n">
+        <v>3</v>
+      </c>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr"/>
@@ -4994,7 +5012,9 @@
       <c r="W39" t="inlineStr"/>
       <c r="X39" t="inlineStr"/>
       <c r="Y39" t="inlineStr"/>
-      <c r="Z39" t="inlineStr"/>
+      <c r="Z39" t="n">
+        <v>1</v>
+      </c>
       <c r="AA39" t="inlineStr"/>
       <c r="AB39" t="n">
         <v>488</v>
@@ -12282,10 +12302,12 @@
       <c r="W39" t="inlineStr"/>
       <c r="X39" t="inlineStr"/>
       <c r="Y39" t="inlineStr"/>
-      <c r="Z39" t="inlineStr"/>
+      <c r="Z39" t="n">
+        <v>41</v>
+      </c>
       <c r="AA39" t="inlineStr"/>
       <c r="AB39" t="n">
-        <v>1459</v>
+        <v>1460</v>
       </c>
     </row>
   </sheetData>

</xml_diff>